<commit_message>
standardize GC data file names
</commit_message>
<xml_diff>
--- a/GC-Data-Raw-R/GC-Data-Rcode/PRACTICE/n2o_analysis_draft.xlsx
+++ b/GC-Data-Raw-R/GC-Data-Rcode/PRACTICE/n2o_analysis_draft.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21620" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="200" yWindow="11280" windowWidth="13760" windowHeight="7880" tabRatio="500" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Vial info" sheetId="1" r:id="rId1"/>
     <sheet name="Chamber Flux Calcs" sheetId="2" r:id="rId2"/>
     <sheet name="Site Summary" sheetId="3" r:id="rId3"/>
+    <sheet name="Stds Info" sheetId="4" r:id="rId4"/>
+    <sheet name="GC Run Names" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="140">
   <si>
     <t>N2Oraw</t>
   </si>
@@ -105,6 +107,342 @@
   </si>
   <si>
     <t>SampleDate</t>
+  </si>
+  <si>
+    <t>Std conc.</t>
+  </si>
+  <si>
+    <t>N2O</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>= air temp, degrees C</t>
+  </si>
+  <si>
+    <t>Mix</t>
+  </si>
+  <si>
+    <t>Standard concentrations for trace gases in ppm.</t>
+  </si>
+  <si>
+    <t>Change standard concentrations in this table only</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> if needed, not in the spreadsheet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aggregate </t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>aggregate</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>Stand 1</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>ppm</t>
+  </si>
+  <si>
+    <t>Stand 2</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>ref ACs</t>
+  </si>
+  <si>
+    <t>Mix 1</t>
+  </si>
+  <si>
+    <t>Mix 2</t>
+  </si>
+  <si>
+    <t>3 N2O</t>
+  </si>
+  <si>
+    <t>High level N2O calibration</t>
+  </si>
+  <si>
+    <t>Slope</t>
+  </si>
+  <si>
+    <t>Pearson's r squared</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>Aggregate slope</t>
+  </si>
+  <si>
+    <t>Aggregate intercept</t>
+  </si>
+  <si>
+    <t>Aggregate r2</t>
+  </si>
+  <si>
+    <t>Low level N2O calibration</t>
+  </si>
+  <si>
+    <t>mix1</t>
+  </si>
+  <si>
+    <t>mix</t>
+  </si>
+  <si>
+    <t>mix2</t>
+  </si>
+  <si>
+    <t>3KCO2</t>
+  </si>
+  <si>
+    <t>High level CO2 calibration</t>
+  </si>
+  <si>
+    <t>Low level CO2 calibration</t>
+  </si>
+  <si>
+    <t>Volume correction</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>Amb1</t>
+  </si>
+  <si>
+    <t>Amb2</t>
+  </si>
+  <si>
+    <t>Amb3</t>
+  </si>
+  <si>
+    <t>Amb4</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Std</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Vial volume (cc)</t>
+  </si>
+  <si>
+    <t>oC</t>
+  </si>
+  <si>
+    <t>Area corrections are linked to these cells.  Change volume values here if needed.</t>
+  </si>
+  <si>
+    <t>Sample volume (cc)</t>
+  </si>
+  <si>
+    <t>Total volume (cc)</t>
+  </si>
+  <si>
+    <t>Time Zero Samples From the Chambers</t>
+  </si>
+  <si>
+    <t>Trip Standard</t>
+  </si>
+  <si>
+    <t>SM-A-20-T0</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>There was no trip standard</t>
+  </si>
+  <si>
+    <t>SM-C-20-T0</t>
+  </si>
+  <si>
+    <t>Mix name</t>
+  </si>
+  <si>
+    <t>M3-A-18-T0</t>
+  </si>
+  <si>
+    <t>M3-B-18-T0</t>
+  </si>
+  <si>
+    <t>Measured</t>
+  </si>
+  <si>
+    <t>Supposed to be</t>
+  </si>
+  <si>
+    <t>M3-C-18-T0</t>
+  </si>
+  <si>
+    <t>M3-D-18-T0</t>
+  </si>
+  <si>
+    <t>M3-E-18-T0</t>
+  </si>
+  <si>
+    <t>M3-A-14-T0</t>
+  </si>
+  <si>
+    <t>plus 1 std</t>
+  </si>
+  <si>
+    <t>M3-B-14-T0</t>
+  </si>
+  <si>
+    <t>minus 1 std</t>
+  </si>
+  <si>
+    <t>M3-C-14-T0</t>
+  </si>
+  <si>
+    <t>M3-D-14-T0</t>
+  </si>
+  <si>
+    <t>M3-E-14-T0</t>
+  </si>
+  <si>
+    <t>SM-A-14-T0</t>
+  </si>
+  <si>
+    <t>SM-B-14-T0</t>
+  </si>
+  <si>
+    <t>SM-C-14-T0</t>
+  </si>
+  <si>
+    <t>SM-D-14-T0</t>
+  </si>
+  <si>
+    <t>SM-E-14-T0</t>
+  </si>
+  <si>
+    <t>SD-A-12-T0</t>
+  </si>
+  <si>
+    <t>SD-B-12-T0</t>
+  </si>
+  <si>
+    <t>SD-C-12-T0</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>upper limit</t>
+  </si>
+  <si>
+    <t>lower limit</t>
+  </si>
+  <si>
+    <t>no std dev</t>
+  </si>
+  <si>
+    <t>Std1</t>
+  </si>
+  <si>
+    <t>Std2</t>
+  </si>
+  <si>
+    <t>Std3</t>
+  </si>
+  <si>
+    <t>airtemp</t>
+  </si>
+  <si>
+    <t>20131104_AA</t>
+  </si>
+  <si>
+    <t>20131105_BB</t>
+  </si>
+  <si>
+    <t>20131105_U</t>
+  </si>
+  <si>
+    <t>20131106_V</t>
+  </si>
+  <si>
+    <t>20131106_W</t>
+  </si>
+  <si>
+    <t>20131107_X</t>
+  </si>
+  <si>
+    <t>20131107_Y</t>
+  </si>
+  <si>
+    <t>20131107_Z</t>
+  </si>
+  <si>
+    <t>20140114_V</t>
+  </si>
+  <si>
+    <t>20140114_W</t>
+  </si>
+  <si>
+    <t>20140113_X</t>
+  </si>
+  <si>
+    <t>20140310_H</t>
+  </si>
+  <si>
+    <t>20140310_U</t>
+  </si>
+  <si>
+    <t>20140311_W</t>
+  </si>
+  <si>
+    <t>20140311_X</t>
+  </si>
+  <si>
+    <t>20140312_Y</t>
+  </si>
+  <si>
+    <t>20140313_Z</t>
+  </si>
+  <si>
+    <t>20140416_J</t>
+  </si>
+  <si>
+    <t>20140417_K</t>
+  </si>
+  <si>
+    <t>20140418_M</t>
+  </si>
+  <si>
+    <t>20140417_N</t>
+  </si>
+  <si>
+    <t>20140418_P</t>
+  </si>
+  <si>
+    <t>20140416_V</t>
+  </si>
+  <si>
+    <t>20140606_Leak0</t>
+  </si>
+  <si>
+    <t>20140613_Leak1</t>
+  </si>
+  <si>
+    <t>20140605_Trav</t>
   </si>
 </sst>
 </file>
@@ -160,7 +498,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -214,13 +552,114 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="153">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -247,6 +686,56 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -273,6 +762,56 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -604,7 +1143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -790,4 +1329,1389 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q93"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="C2">
+        <v>600</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="H2">
+        <v>600</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3">
+        <v>1.57</v>
+      </c>
+      <c r="C3">
+        <v>1000</v>
+      </c>
+      <c r="G3">
+        <v>1.57</v>
+      </c>
+      <c r="H3">
+        <v>1000</v>
+      </c>
+      <c r="K3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>3000</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>3000</v>
+      </c>
+      <c r="K4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" t="s">
+        <v>38</v>
+      </c>
+      <c r="P5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" t="s">
+        <v>44</v>
+      </c>
+      <c r="O6" t="s">
+        <v>42</v>
+      </c>
+      <c r="P6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7">
+        <v>15.205862499999995</v>
+      </c>
+      <c r="H7">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="J7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7">
+        <v>15.205862499999995</v>
+      </c>
+      <c r="L7">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="M7">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="N7">
+        <v>15.205862499999995</v>
+      </c>
+      <c r="O7">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="P7">
+        <v>15.205862499999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="F8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8">
+        <v>84.736512499999989</v>
+      </c>
+      <c r="H8">
+        <v>1.57</v>
+      </c>
+      <c r="J8" t="s">
+        <v>47</v>
+      </c>
+      <c r="K8">
+        <v>84.736512499999989</v>
+      </c>
+      <c r="L8">
+        <v>1.57</v>
+      </c>
+      <c r="M8">
+        <v>1.57</v>
+      </c>
+      <c r="N8">
+        <v>84.736512499999989</v>
+      </c>
+      <c r="O8">
+        <v>1.57</v>
+      </c>
+      <c r="P8">
+        <v>84.736512499999989</v>
+      </c>
+      <c r="Q8">
+        <v>84.736512499999989</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9">
+        <v>140.52021249999999</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9">
+        <v>140.52021249999999</v>
+      </c>
+      <c r="L9">
+        <v>3</v>
+      </c>
+      <c r="M9">
+        <v>3</v>
+      </c>
+      <c r="N9">
+        <v>140.52021249999999</v>
+      </c>
+      <c r="O9">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="P9">
+        <v>15.205862499999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+      <c r="M10">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="N10">
+        <v>15.205862499999995</v>
+      </c>
+      <c r="O10">
+        <v>1.57</v>
+      </c>
+      <c r="P10">
+        <v>84.736512499999989</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11">
+        <v>2.1404994261226374E-2</v>
+      </c>
+      <c r="J11" t="s">
+        <v>50</v>
+      </c>
+      <c r="L11">
+        <v>2.1404994261226374E-2</v>
+      </c>
+      <c r="M11">
+        <v>1.57</v>
+      </c>
+      <c r="N11">
+        <v>84.736512499999989</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12">
+        <v>0.99048950439700612</v>
+      </c>
+      <c r="J12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12">
+        <v>0.99048950439700612</v>
+      </c>
+      <c r="M12">
+        <v>3</v>
+      </c>
+      <c r="N12">
+        <v>140.52021249999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="F13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13">
+        <v>-9.203343515904816E-2</v>
+      </c>
+      <c r="J13" t="s">
+        <v>52</v>
+      </c>
+      <c r="L13">
+        <v>-9.203343515904816E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="J14" t="s">
+        <v>53</v>
+      </c>
+      <c r="L14">
+        <v>2.1404994261226367E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="J15" t="s">
+        <v>54</v>
+      </c>
+      <c r="L15">
+        <v>-9.2033435159047494E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="J16" t="s">
+        <v>55</v>
+      </c>
+      <c r="L16">
+        <v>0.99048950439700523</v>
+      </c>
+    </row>
+    <row r="17" spans="6:17">
+      <c r="F17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="6:17">
+      <c r="F18" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18">
+        <v>1.8250944008146051E-2</v>
+      </c>
+      <c r="J18" t="s">
+        <v>50</v>
+      </c>
+      <c r="L18">
+        <v>1.8250944008146051E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="6:17">
+      <c r="F19" t="s">
+        <v>51</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="J19" t="s">
+        <v>51</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="6:17">
+      <c r="F20" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20">
+        <v>2.347865491693224E-2</v>
+      </c>
+      <c r="J20" t="s">
+        <v>52</v>
+      </c>
+      <c r="L20">
+        <v>2.347865491693224E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="6:17">
+      <c r="J21" t="s">
+        <v>53</v>
+      </c>
+      <c r="L21">
+        <v>1.8250944008146051E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="6:17">
+      <c r="J22" t="s">
+        <v>54</v>
+      </c>
+      <c r="L22">
+        <v>2.347865491693224E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="6:17">
+      <c r="J23" t="s">
+        <v>55</v>
+      </c>
+      <c r="L23">
+        <v>0.99999999999999978</v>
+      </c>
+    </row>
+    <row r="25" spans="6:17">
+      <c r="F25" t="s">
+        <v>30</v>
+      </c>
+      <c r="M25" t="s">
+        <v>36</v>
+      </c>
+      <c r="N25" t="s">
+        <v>37</v>
+      </c>
+      <c r="O25" t="s">
+        <v>38</v>
+      </c>
+      <c r="P25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="6:17">
+      <c r="F26" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" t="s">
+        <v>41</v>
+      </c>
+      <c r="H26" t="s">
+        <v>42</v>
+      </c>
+      <c r="J26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K26" t="s">
+        <v>41</v>
+      </c>
+      <c r="L26" t="s">
+        <v>42</v>
+      </c>
+      <c r="M26" t="s">
+        <v>42</v>
+      </c>
+      <c r="N26" t="s">
+        <v>44</v>
+      </c>
+      <c r="O26" t="s">
+        <v>42</v>
+      </c>
+      <c r="P26" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="6:17">
+      <c r="F27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27">
+        <v>61.487075000000011</v>
+      </c>
+      <c r="H27">
+        <v>600</v>
+      </c>
+      <c r="J27" t="s">
+        <v>58</v>
+      </c>
+      <c r="K27">
+        <v>61.487075000000011</v>
+      </c>
+      <c r="L27">
+        <v>600</v>
+      </c>
+      <c r="M27">
+        <v>600</v>
+      </c>
+      <c r="N27">
+        <v>61.487075000000011</v>
+      </c>
+      <c r="O27">
+        <v>600</v>
+      </c>
+      <c r="P27">
+        <v>61.487075000000011</v>
+      </c>
+    </row>
+    <row r="28" spans="6:17">
+      <c r="F28" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="J28" t="s">
+        <v>59</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>61.487075000000011</v>
+      </c>
+    </row>
+    <row r="29" spans="6:17">
+      <c r="F29" t="s">
+        <v>60</v>
+      </c>
+      <c r="G29">
+        <v>259.881775</v>
+      </c>
+      <c r="H29">
+        <v>3000</v>
+      </c>
+      <c r="J29" t="s">
+        <v>60</v>
+      </c>
+      <c r="K29">
+        <v>259.881775</v>
+      </c>
+      <c r="L29">
+        <v>3000</v>
+      </c>
+      <c r="M29">
+        <v>3000</v>
+      </c>
+      <c r="N29">
+        <v>259.881775</v>
+      </c>
+      <c r="O29">
+        <v>600</v>
+      </c>
+      <c r="P29">
+        <v>61.487075000000011</v>
+      </c>
+    </row>
+    <row r="30" spans="6:17">
+      <c r="F30" t="s">
+        <v>61</v>
+      </c>
+      <c r="M30">
+        <v>600</v>
+      </c>
+      <c r="N30">
+        <v>61.487075000000011</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="6:17">
+      <c r="F31" t="s">
+        <v>50</v>
+      </c>
+      <c r="H31">
+        <v>11.679516506502203</v>
+      </c>
+      <c r="J31" t="s">
+        <v>50</v>
+      </c>
+      <c r="L31">
+        <v>11.679516506502203</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="6:17">
+      <c r="F32" t="s">
+        <v>51</v>
+      </c>
+      <c r="H32">
+        <v>0.99854061132806404</v>
+      </c>
+      <c r="J32" t="s">
+        <v>51</v>
+      </c>
+      <c r="L32">
+        <v>0.99854061132806404</v>
+      </c>
+      <c r="M32">
+        <v>3000</v>
+      </c>
+      <c r="N32">
+        <v>259.881775</v>
+      </c>
+    </row>
+    <row r="33" spans="6:12">
+      <c r="F33" t="s">
+        <v>52</v>
+      </c>
+      <c r="H33">
+        <v>-51.144262750210146</v>
+      </c>
+      <c r="J33" t="s">
+        <v>52</v>
+      </c>
+      <c r="L33">
+        <v>-51.144262750210146</v>
+      </c>
+    </row>
+    <row r="34" spans="6:12">
+      <c r="J34" t="s">
+        <v>53</v>
+      </c>
+      <c r="L34">
+        <v>11.679516506502203</v>
+      </c>
+    </row>
+    <row r="35" spans="6:12">
+      <c r="J35" t="s">
+        <v>54</v>
+      </c>
+      <c r="L35">
+        <v>-51.144262750210146</v>
+      </c>
+    </row>
+    <row r="36" spans="6:12">
+      <c r="J36" t="s">
+        <v>55</v>
+      </c>
+      <c r="L36">
+        <v>0.99854061132806382</v>
+      </c>
+    </row>
+    <row r="37" spans="6:12">
+      <c r="F37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="6:12">
+      <c r="F38" t="s">
+        <v>50</v>
+      </c>
+      <c r="H38">
+        <v>9.7581483588217512</v>
+      </c>
+      <c r="J38" t="s">
+        <v>50</v>
+      </c>
+      <c r="L38">
+        <v>9.7581483588217512</v>
+      </c>
+    </row>
+    <row r="39" spans="6:12">
+      <c r="F39" t="s">
+        <v>51</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="J39" t="s">
+        <v>51</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="6:12">
+      <c r="F40" t="s">
+        <v>52</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="J40" t="s">
+        <v>52</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="6:12">
+      <c r="J41" t="s">
+        <v>53</v>
+      </c>
+      <c r="L41">
+        <v>9.7581483588217512</v>
+      </c>
+    </row>
+    <row r="42" spans="6:12">
+      <c r="J42" t="s">
+        <v>54</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="6:12">
+      <c r="J43" t="s">
+        <v>55</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="6:12">
+      <c r="F46" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="6:12">
+      <c r="F47" t="s">
+        <v>64</v>
+      </c>
+      <c r="G47" t="s">
+        <v>29</v>
+      </c>
+      <c r="H47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="6:12">
+      <c r="F48" t="s">
+        <v>65</v>
+      </c>
+      <c r="G48">
+        <v>17.591200000000001</v>
+      </c>
+      <c r="H48">
+        <v>55.022799999999997</v>
+      </c>
+    </row>
+    <row r="49" spans="6:11">
+      <c r="F49" t="s">
+        <v>66</v>
+      </c>
+      <c r="G49">
+        <v>17.858799999999999</v>
+      </c>
+      <c r="H49">
+        <v>55.35</v>
+      </c>
+    </row>
+    <row r="50" spans="6:11">
+      <c r="F50" t="s">
+        <v>67</v>
+      </c>
+      <c r="G50">
+        <v>17.258400000000002</v>
+      </c>
+      <c r="H50">
+        <v>56.294400000000003</v>
+      </c>
+    </row>
+    <row r="51" spans="6:11">
+      <c r="F51" t="s">
+        <v>68</v>
+      </c>
+      <c r="G51">
+        <v>17.5822</v>
+      </c>
+      <c r="H51">
+        <v>56.169199999999996</v>
+      </c>
+    </row>
+    <row r="53" spans="6:11">
+      <c r="F53" t="s">
+        <v>69</v>
+      </c>
+      <c r="G53">
+        <v>17.572650000000003</v>
+      </c>
+      <c r="H53">
+        <v>55.709099999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="6:11">
+      <c r="F54" t="s">
+        <v>70</v>
+      </c>
+      <c r="G54">
+        <v>0.2456760672104619</v>
+      </c>
+      <c r="H54">
+        <v>0.62027644374638968</v>
+      </c>
+    </row>
+    <row r="55" spans="6:11">
+      <c r="F55" t="s">
+        <v>71</v>
+      </c>
+      <c r="G55">
+        <v>4</v>
+      </c>
+      <c r="H55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="6:11">
+      <c r="F57" t="s">
+        <v>72</v>
+      </c>
+      <c r="H57">
+        <v>9</v>
+      </c>
+      <c r="I57">
+        <v>20</v>
+      </c>
+      <c r="J57" t="s">
+        <v>73</v>
+      </c>
+      <c r="K57" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="58" spans="6:11">
+      <c r="F58" t="s">
+        <v>75</v>
+      </c>
+      <c r="H58">
+        <v>12</v>
+      </c>
+      <c r="I58">
+        <v>12.204673375405083</v>
+      </c>
+    </row>
+    <row r="59" spans="6:11">
+      <c r="F59" t="s">
+        <v>76</v>
+      </c>
+      <c r="H59">
+        <v>21</v>
+      </c>
+      <c r="I59">
+        <v>21.204673375405083</v>
+      </c>
+    </row>
+    <row r="65" spans="6:14">
+      <c r="F65" t="s">
+        <v>77</v>
+      </c>
+      <c r="K65" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" spans="6:14">
+      <c r="F67" t="s">
+        <v>79</v>
+      </c>
+      <c r="G67">
+        <v>0.3469595977504093</v>
+      </c>
+      <c r="H67">
+        <v>363.98806275848921</v>
+      </c>
+      <c r="K67" t="s">
+        <v>80</v>
+      </c>
+      <c r="L67" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="68" spans="6:14">
+      <c r="F68" t="s">
+        <v>82</v>
+      </c>
+      <c r="G68">
+        <v>0.32901196435349778</v>
+      </c>
+      <c r="H68">
+        <v>449.80934194305291</v>
+      </c>
+      <c r="K68" t="s">
+        <v>83</v>
+      </c>
+      <c r="L68" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="69" spans="6:14">
+      <c r="F69" t="s">
+        <v>84</v>
+      </c>
+      <c r="G69">
+        <v>0.38596874722899699</v>
+      </c>
+      <c r="H69">
+        <v>450.31118111015354</v>
+      </c>
+    </row>
+    <row r="70" spans="6:14">
+      <c r="F70" t="s">
+        <v>85</v>
+      </c>
+      <c r="G70">
+        <v>0.37195944610752074</v>
+      </c>
+      <c r="H70">
+        <v>358.23725716793138</v>
+      </c>
+      <c r="K70" t="s">
+        <v>86</v>
+      </c>
+      <c r="M70" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="71" spans="6:14">
+      <c r="F71" t="s">
+        <v>88</v>
+      </c>
+      <c r="G71">
+        <v>0.36594096409562366</v>
+      </c>
+      <c r="H71">
+        <v>534.99314975319169</v>
+      </c>
+      <c r="K71" t="s">
+        <v>29</v>
+      </c>
+      <c r="L71" t="s">
+        <v>30</v>
+      </c>
+      <c r="M71" t="s">
+        <v>29</v>
+      </c>
+      <c r="N71" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="6:14">
+      <c r="F72" t="s">
+        <v>89</v>
+      </c>
+      <c r="G72">
+        <v>0.35987174672430045</v>
+      </c>
+      <c r="H72">
+        <v>433.15370688360696</v>
+      </c>
+      <c r="K72" t="s">
+        <v>42</v>
+      </c>
+      <c r="L72" t="s">
+        <v>42</v>
+      </c>
+      <c r="M72" t="s">
+        <v>42</v>
+      </c>
+      <c r="N72" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73" spans="6:14">
+      <c r="F73" t="s">
+        <v>90</v>
+      </c>
+      <c r="G73">
+        <v>0.37176284658974534</v>
+      </c>
+      <c r="H73">
+        <v>461.76193021352259</v>
+      </c>
+      <c r="K73">
+        <v>-0.21302558999301613</v>
+      </c>
+      <c r="L73">
+        <v>-400.87586239607526</v>
+      </c>
+      <c r="M73">
+        <v>0</v>
+      </c>
+      <c r="N73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="6:14">
+      <c r="F74" t="s">
+        <v>91</v>
+      </c>
+      <c r="G74">
+        <v>0.34229828660315481</v>
+      </c>
+      <c r="H74">
+        <v>430.19014315356708</v>
+      </c>
+      <c r="J74" t="s">
+        <v>92</v>
+      </c>
+      <c r="K74">
+        <v>-0.21633205957888144</v>
+      </c>
+      <c r="L74">
+        <v>-405.33929573660328</v>
+      </c>
+    </row>
+    <row r="75" spans="6:14">
+      <c r="F75" t="s">
+        <v>93</v>
+      </c>
+      <c r="G75">
+        <v>0.31738722512503875</v>
+      </c>
+      <c r="H75">
+        <v>434.5303737879504</v>
+      </c>
+      <c r="J75" t="s">
+        <v>94</v>
+      </c>
+      <c r="K75">
+        <v>-0.20971912040715085</v>
+      </c>
+      <c r="L75">
+        <v>-396.41242905554731</v>
+      </c>
+    </row>
+    <row r="76" spans="6:14">
+      <c r="F76" t="s">
+        <v>95</v>
+      </c>
+      <c r="G76">
+        <v>0.32431260168667386</v>
+      </c>
+      <c r="H76">
+        <v>448.93790501099318</v>
+      </c>
+    </row>
+    <row r="77" spans="6:14">
+      <c r="F77" t="s">
+        <v>96</v>
+      </c>
+      <c r="G77">
+        <v>0.36424132955485594</v>
+      </c>
+      <c r="H77">
+        <v>458.24566523863541</v>
+      </c>
+    </row>
+    <row r="78" spans="6:14">
+      <c r="F78" t="s">
+        <v>97</v>
+      </c>
+      <c r="G78">
+        <v>0.36579509993727405</v>
+      </c>
+      <c r="H78">
+        <v>511.26429508177409</v>
+      </c>
+    </row>
+    <row r="79" spans="6:14">
+      <c r="F79" t="s">
+        <v>98</v>
+      </c>
+      <c r="G79">
+        <v>0.37984245257831967</v>
+      </c>
+      <c r="H79">
+        <v>559.1356826569488</v>
+      </c>
+    </row>
+    <row r="80" spans="6:14">
+      <c r="F80" t="s">
+        <v>99</v>
+      </c>
+      <c r="G80">
+        <v>0.41219892805218639</v>
+      </c>
+      <c r="H80">
+        <v>595.42407972661283</v>
+      </c>
+    </row>
+    <row r="81" spans="6:8">
+      <c r="F81" t="s">
+        <v>100</v>
+      </c>
+      <c r="G81">
+        <v>0.40834938265574638</v>
+      </c>
+      <c r="H81">
+        <v>705.91758281214425</v>
+      </c>
+    </row>
+    <row r="82" spans="6:8">
+      <c r="F82" t="s">
+        <v>101</v>
+      </c>
+      <c r="G82">
+        <v>0.35547045429410379</v>
+      </c>
+      <c r="H82">
+        <v>421.91996931195717</v>
+      </c>
+    </row>
+    <row r="83" spans="6:8">
+      <c r="F83" t="s">
+        <v>102</v>
+      </c>
+      <c r="G83">
+        <v>0.3753143217495582</v>
+      </c>
+      <c r="H83">
+        <v>510.01647877438893</v>
+      </c>
+    </row>
+    <row r="84" spans="6:8">
+      <c r="F84" t="s">
+        <v>103</v>
+      </c>
+      <c r="G84">
+        <v>0.39995902259068844</v>
+      </c>
+      <c r="H84">
+        <v>573.30585751717354</v>
+      </c>
+    </row>
+    <row r="85" spans="6:8">
+      <c r="F85" t="s">
+        <v>104</v>
+      </c>
+      <c r="G85">
+        <v>0.39478401592924678</v>
+      </c>
+      <c r="H85">
+        <v>541.25596692639942</v>
+      </c>
+    </row>
+    <row r="86" spans="6:8">
+      <c r="F86" t="s">
+        <v>105</v>
+      </c>
+      <c r="G86">
+        <v>0.39335074202546516</v>
+      </c>
+      <c r="H86">
+        <v>528.20475777660135</v>
+      </c>
+    </row>
+    <row r="89" spans="6:8">
+      <c r="G89">
+        <v>0.36823895878162033</v>
+      </c>
+      <c r="H89">
+        <v>488.53016938025468</v>
+      </c>
+    </row>
+    <row r="90" spans="6:8">
+      <c r="F90" t="s">
+        <v>106</v>
+      </c>
+      <c r="G90">
+        <v>7.331461098869517E-2</v>
+      </c>
+      <c r="H90">
+        <v>0.1698501751512545</v>
+      </c>
+    </row>
+    <row r="91" spans="6:8">
+      <c r="F91" t="s">
+        <v>107</v>
+      </c>
+      <c r="G91">
+        <v>0.42223355080953362</v>
+      </c>
+      <c r="H91">
+        <v>654.48403905207124</v>
+      </c>
+    </row>
+    <row r="92" spans="6:8">
+      <c r="F92" t="s">
+        <v>108</v>
+      </c>
+      <c r="G92">
+        <v>0.31424436675370704</v>
+      </c>
+      <c r="H92">
+        <v>322.57629970843811</v>
+      </c>
+    </row>
+    <row r="93" spans="6:8">
+      <c r="F93" t="s">
+        <v>109</v>
+      </c>
+      <c r="G93">
+        <v>2</v>
+      </c>
+      <c r="H93">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finished entering all GC runsheets
and standardized all file names for runsheets, ecd, fid and tcd files -
woohoo!
</commit_message>
<xml_diff>
--- a/GC-Data-Raw-R/GC-Data-Rcode/PRACTICE/n2o_analysis_draft.xlsx
+++ b/GC-Data-Raw-R/GC-Data-Rcode/PRACTICE/n2o_analysis_draft.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="11280" windowWidth="13760" windowHeight="7880" tabRatio="500" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="200" yWindow="11280" windowWidth="16240" windowHeight="7880" tabRatio="850" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Vial info" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Site Summary" sheetId="3" r:id="rId3"/>
     <sheet name="Stds Info" sheetId="4" r:id="rId4"/>
     <sheet name="GC Run Names" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="326">
   <si>
     <t>N2Oraw</t>
   </si>
@@ -443,13 +444,571 @@
   </si>
   <si>
     <t>20140605_Trav</t>
+  </si>
+  <si>
+    <t>Mix1</t>
+  </si>
+  <si>
+    <t>Mix2</t>
+  </si>
+  <si>
+    <t>3N2O</t>
+  </si>
+  <si>
+    <t>10N2O</t>
+  </si>
+  <si>
+    <t>amb</t>
+  </si>
+  <si>
+    <t>F2-A-25-T0</t>
+  </si>
+  <si>
+    <t>F2-A-25-T15</t>
+  </si>
+  <si>
+    <t>F2-A-25-T30</t>
+  </si>
+  <si>
+    <t>F2-A-25-T45</t>
+  </si>
+  <si>
+    <t>F2-C-25-T0</t>
+  </si>
+  <si>
+    <t>F2-C-25-T15</t>
+  </si>
+  <si>
+    <t>F2-C-25-T30</t>
+  </si>
+  <si>
+    <t>F2-C-25-T45</t>
+  </si>
+  <si>
+    <t>F2-B-25-T0</t>
+  </si>
+  <si>
+    <t>F2-B-25-T15</t>
+  </si>
+  <si>
+    <t>M3-C-25-T30</t>
+  </si>
+  <si>
+    <t>M3-C-25-T45</t>
+  </si>
+  <si>
+    <t>M3-D-25-T0</t>
+  </si>
+  <si>
+    <t>M3-D-25-T15</t>
+  </si>
+  <si>
+    <t>M3-D-25-T30</t>
+  </si>
+  <si>
+    <t>M3-D-25-T45</t>
+  </si>
+  <si>
+    <t>M3-E-25-T0</t>
+  </si>
+  <si>
+    <t>M3-E-25-T15</t>
+  </si>
+  <si>
+    <t>M3-E-25-T30</t>
+  </si>
+  <si>
+    <t>M3-E-25-T45</t>
+  </si>
+  <si>
+    <t>M3-A-25-T0</t>
+  </si>
+  <si>
+    <t>M3-A-25-T15</t>
+  </si>
+  <si>
+    <t>M3-A-25-T30</t>
+  </si>
+  <si>
+    <t>M3-A-25-T45</t>
+  </si>
+  <si>
+    <t>M3-B-25-T0</t>
+  </si>
+  <si>
+    <t>M3-B-25-T15</t>
+  </si>
+  <si>
+    <t>M3-B-25-T30</t>
+  </si>
+  <si>
+    <t>M3-B-25-T45</t>
+  </si>
+  <si>
+    <t>M3-C-25-T0</t>
+  </si>
+  <si>
+    <t>M3-C-25-T15</t>
+  </si>
+  <si>
+    <t>SM-C-24-T30</t>
+  </si>
+  <si>
+    <t>SM-C-24-T45</t>
+  </si>
+  <si>
+    <t>SM-D-24-T0</t>
+  </si>
+  <si>
+    <t>SM-D-24-T15</t>
+  </si>
+  <si>
+    <t>SM-D-24-T30</t>
+  </si>
+  <si>
+    <t>SM-D-24-T45</t>
+  </si>
+  <si>
+    <t>SM-E-24-T0</t>
+  </si>
+  <si>
+    <t>SM-E-24-T15</t>
+  </si>
+  <si>
+    <t>SM-E-24-T30</t>
+  </si>
+  <si>
+    <t>SM-E-24-T45</t>
+  </si>
+  <si>
+    <t>SM-A-24-T0</t>
+  </si>
+  <si>
+    <t>SM-A-24-T15</t>
+  </si>
+  <si>
+    <t>SM-A-24-T30</t>
+  </si>
+  <si>
+    <t>SM-A-24-T45</t>
+  </si>
+  <si>
+    <t>SM-B-24-T0</t>
+  </si>
+  <si>
+    <t>SM-B-24-T15</t>
+  </si>
+  <si>
+    <t>SM-B-24-T30</t>
+  </si>
+  <si>
+    <t>SM-B-24-T45</t>
+  </si>
+  <si>
+    <t>SM-C-24-T0</t>
+  </si>
+  <si>
+    <t>SM-C-24-T15</t>
+  </si>
+  <si>
+    <t>M3-C-21-T30</t>
+  </si>
+  <si>
+    <t>M3-C-21-T45</t>
+  </si>
+  <si>
+    <t>M3-D-21-T0</t>
+  </si>
+  <si>
+    <t>M3-D-21-T15</t>
+  </si>
+  <si>
+    <t>M3-D-21-T30</t>
+  </si>
+  <si>
+    <t>M3-D-21-T45</t>
+  </si>
+  <si>
+    <t>M3-E-21-T0</t>
+  </si>
+  <si>
+    <t>M3-E-21-T15</t>
+  </si>
+  <si>
+    <t>M3-E-21-T30</t>
+  </si>
+  <si>
+    <t>M3-E-21-T45</t>
+  </si>
+  <si>
+    <t>M3-A-21-T0</t>
+  </si>
+  <si>
+    <t>M3-A-21-T15</t>
+  </si>
+  <si>
+    <t>M3-A-21-T30</t>
+  </si>
+  <si>
+    <t>M3-A-21-T45</t>
+  </si>
+  <si>
+    <t>M3-B-21-T0</t>
+  </si>
+  <si>
+    <t>M3-B-21-T15</t>
+  </si>
+  <si>
+    <t>M3-B-21-T30</t>
+  </si>
+  <si>
+    <t>M3-B-21-T45</t>
+  </si>
+  <si>
+    <t>M3-C-21-T0</t>
+  </si>
+  <si>
+    <t>M3-C-21-T15</t>
+  </si>
+  <si>
+    <t>F2-C-20-T30</t>
+  </si>
+  <si>
+    <t>F2-C-20-T45</t>
+  </si>
+  <si>
+    <t>F2-D-20-T0</t>
+  </si>
+  <si>
+    <t>F2-D-20-T15</t>
+  </si>
+  <si>
+    <t>F2-D-20-T30</t>
+  </si>
+  <si>
+    <t>F2-D-20-T45</t>
+  </si>
+  <si>
+    <t>F2-E-20-T0</t>
+  </si>
+  <si>
+    <t>F2-E-20-T15</t>
+  </si>
+  <si>
+    <t>F2-E-20-T30</t>
+  </si>
+  <si>
+    <t>F2-E-20-T45</t>
+  </si>
+  <si>
+    <t>F2-A-20-T0</t>
+  </si>
+  <si>
+    <t>F2-A-20-T15</t>
+  </si>
+  <si>
+    <t>F2-A-20-T30</t>
+  </si>
+  <si>
+    <t>F2-A-20-T45</t>
+  </si>
+  <si>
+    <t>F2-B-20-T0</t>
+  </si>
+  <si>
+    <t>F2-B-20-T15</t>
+  </si>
+  <si>
+    <t>F2-B-20-T30</t>
+  </si>
+  <si>
+    <t>F2-B-20-T45</t>
+  </si>
+  <si>
+    <t>F2-C-20-T0</t>
+  </si>
+  <si>
+    <t>F2-C-20-T15</t>
+  </si>
+  <si>
+    <t>trav_dummy</t>
+  </si>
+  <si>
+    <t>M1-A-13-T0</t>
+  </si>
+  <si>
+    <t>M1-A-13-T15</t>
+  </si>
+  <si>
+    <t>M1-A-13-T30</t>
+  </si>
+  <si>
+    <t>M1-A-13-T45</t>
+  </si>
+  <si>
+    <t>M1-B-13-T0</t>
+  </si>
+  <si>
+    <t>M1-B-13-T15</t>
+  </si>
+  <si>
+    <t>M1-B-13-T30</t>
+  </si>
+  <si>
+    <t>M1-B-13-T45</t>
+  </si>
+  <si>
+    <t>M1-C-13-T0</t>
+  </si>
+  <si>
+    <t>M1-C-13-T15</t>
+  </si>
+  <si>
+    <t>M1-C-13-T30</t>
+  </si>
+  <si>
+    <t>M1-C-13-T45</t>
+  </si>
+  <si>
+    <t>M1-D-13-T0</t>
+  </si>
+  <si>
+    <t>M1-D-13-T15</t>
+  </si>
+  <si>
+    <t>M1-D-13-T30</t>
+  </si>
+  <si>
+    <t>M1-D-13-T45</t>
+  </si>
+  <si>
+    <t>M1-E-13-T0</t>
+  </si>
+  <si>
+    <t>M1-E-13-T15</t>
+  </si>
+  <si>
+    <t>M1-E-13-T30</t>
+  </si>
+  <si>
+    <t>M1-E-13-T45</t>
+  </si>
+  <si>
+    <t>SM-A-13-T0</t>
+  </si>
+  <si>
+    <t>SM-A-13-T15</t>
+  </si>
+  <si>
+    <t>SM-A-13-T30</t>
+  </si>
+  <si>
+    <t>SM-A-13-T45</t>
+  </si>
+  <si>
+    <t>SM-B-13-T0</t>
+  </si>
+  <si>
+    <t>SM-B-13-T15</t>
+  </si>
+  <si>
+    <t>SM-B-13-T30</t>
+  </si>
+  <si>
+    <t>SM-B-13-T45</t>
+  </si>
+  <si>
+    <t>SM-C-13-T0</t>
+  </si>
+  <si>
+    <t>SM-C-13-T15</t>
+  </si>
+  <si>
+    <t>SM-C-13-T30</t>
+  </si>
+  <si>
+    <t>SM-C-13-T45</t>
+  </si>
+  <si>
+    <t>SM-D-13-T0</t>
+  </si>
+  <si>
+    <t>SM-D-13-T15</t>
+  </si>
+  <si>
+    <t>SM-D-13-T30</t>
+  </si>
+  <si>
+    <t>SM-D-13-T45</t>
+  </si>
+  <si>
+    <t>SM-E-13-T0</t>
+  </si>
+  <si>
+    <t>SM-E-13-T15</t>
+  </si>
+  <si>
+    <t>SM-E-13-T30</t>
+  </si>
+  <si>
+    <t>SM-E-13-T45</t>
+  </si>
+  <si>
+    <t>M2-A-18-T0</t>
+  </si>
+  <si>
+    <t>M2-A-18-T15</t>
+  </si>
+  <si>
+    <t>M2-A-18-T30</t>
+  </si>
+  <si>
+    <t>M2-A-18-T45</t>
+  </si>
+  <si>
+    <t>M2-B-18-T0</t>
+  </si>
+  <si>
+    <t>M2-B-18-T15</t>
+  </si>
+  <si>
+    <t>M2-B-18-T30</t>
+  </si>
+  <si>
+    <t>M2-B-18-T45</t>
+  </si>
+  <si>
+    <t>M2-C-18-T0</t>
+  </si>
+  <si>
+    <t>M2-C-18-T15</t>
+  </si>
+  <si>
+    <t>M2-C-18-T30</t>
+  </si>
+  <si>
+    <t>M2-C-18-T45</t>
+  </si>
+  <si>
+    <t>M2-D-18-T0</t>
+  </si>
+  <si>
+    <t>M2-D-18-T15</t>
+  </si>
+  <si>
+    <t>M2-D-18-T30</t>
+  </si>
+  <si>
+    <t>M2-D-18-T45</t>
+  </si>
+  <si>
+    <t>M2-E-18-T0</t>
+  </si>
+  <si>
+    <t>M2-E-18-T15</t>
+  </si>
+  <si>
+    <t>M2-E-18-T30</t>
+  </si>
+  <si>
+    <t>M2-E-18-T45</t>
+  </si>
+  <si>
+    <t>SM-A-18-T0</t>
+  </si>
+  <si>
+    <t>SM-A-18-T15</t>
+  </si>
+  <si>
+    <t>SM-A-18-T30</t>
+  </si>
+  <si>
+    <t>SM-A-18-T45</t>
+  </si>
+  <si>
+    <t>SM-B-18-T0</t>
+  </si>
+  <si>
+    <t>SM-B-18-T15</t>
+  </si>
+  <si>
+    <t>SM-B-18-T30</t>
+  </si>
+  <si>
+    <t>SM-B-18-T45</t>
+  </si>
+  <si>
+    <t>SM-C-18-T0</t>
+  </si>
+  <si>
+    <t>SM-C-18-T15</t>
+  </si>
+  <si>
+    <t>SM-C-18-T30</t>
+  </si>
+  <si>
+    <t>SM-C-18-T45</t>
+  </si>
+  <si>
+    <t>SM-D-18-T0</t>
+  </si>
+  <si>
+    <t>SM-D-18-T15</t>
+  </si>
+  <si>
+    <t>SM-D-18-T30</t>
+  </si>
+  <si>
+    <t>SM-D-18-T45</t>
+  </si>
+  <si>
+    <t>SM-E-18-T0</t>
+  </si>
+  <si>
+    <t>SM-E-18-T15</t>
+  </si>
+  <si>
+    <t>SM-E-18-T30</t>
+  </si>
+  <si>
+    <t>SM-E-18-T45</t>
+  </si>
+  <si>
+    <t>M1-A-10-T0</t>
+  </si>
+  <si>
+    <t>M1-A-10-T15</t>
+  </si>
+  <si>
+    <t>M1-A-10-T30</t>
+  </si>
+  <si>
+    <t>M1-A-10-T45</t>
+  </si>
+  <si>
+    <t>M1-B-10-T0</t>
+  </si>
+  <si>
+    <t>M1-B-10-T15</t>
+  </si>
+  <si>
+    <t>M1-B-10-T30</t>
+  </si>
+  <si>
+    <t>M1-B-10-T45</t>
+  </si>
+  <si>
+    <t>M1-C-10-T0</t>
+  </si>
+  <si>
+    <t>M1-C-10-T15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -480,6 +1039,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -498,7 +1062,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="153">
+  <cellStyleXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -652,14 +1216,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="153">
+  <cellStyles count="157">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -736,6 +1306,8 @@
     <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -812,6 +1384,8 @@
     <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2566,7 +3140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -2714,4 +3288,834 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D1:F101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="12.1640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="4:6">
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="4:6">
+      <c r="D2" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="4:6">
+      <c r="D3" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="4:6">
+      <c r="D4" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6">
+      <c r="D5" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6">
+      <c r="D6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6">
+      <c r="D7" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6">
+      <c r="D8" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6">
+      <c r="D9" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6">
+      <c r="D10" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6">
+      <c r="D11" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6">
+      <c r="D12" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="13" spans="4:6">
+      <c r="D13" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6">
+      <c r="D14" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6">
+      <c r="D15" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="16" spans="4:6">
+      <c r="D16" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6">
+      <c r="D17" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6">
+      <c r="D18" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6">
+      <c r="D19" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6">
+      <c r="D20" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6">
+      <c r="D21" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6">
+      <c r="D22" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6">
+      <c r="D23" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6">
+      <c r="D24" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="25" spans="4:6">
+      <c r="D25" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="26" spans="4:6">
+      <c r="D26" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="27" spans="4:6">
+      <c r="D27" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="28" spans="4:6">
+      <c r="D28" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="29" spans="4:6">
+      <c r="D29" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="30" spans="4:6">
+      <c r="D30" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="31" spans="4:6">
+      <c r="D31" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="32" spans="4:6">
+      <c r="D32" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6">
+      <c r="D33" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6">
+      <c r="D34" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6">
+      <c r="D35" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6">
+      <c r="D36" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6">
+      <c r="D37" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6">
+      <c r="D38" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6">
+      <c r="D39" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6">
+      <c r="D40" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6">
+      <c r="D41" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="42" spans="4:6">
+      <c r="D42" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="43" spans="4:6">
+      <c r="D43" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="44" spans="4:6">
+      <c r="D44" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="45" spans="4:6">
+      <c r="D45" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="46" spans="4:6">
+      <c r="D46" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="47" spans="4:6">
+      <c r="D47" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="48" spans="4:6">
+      <c r="D48" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="49" spans="4:6">
+      <c r="D49" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="50" spans="4:6">
+      <c r="D50" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="51" spans="4:6">
+      <c r="D51" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="52" spans="4:6">
+      <c r="D52" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="53" spans="4:6">
+      <c r="D53" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="54" spans="4:6">
+      <c r="D54" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="55" spans="4:6">
+      <c r="D55" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="56" spans="4:6">
+      <c r="D56" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="57" spans="4:6">
+      <c r="D57" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="58" spans="4:6">
+      <c r="D58" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="59" spans="4:6">
+      <c r="D59" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="60" spans="4:6">
+      <c r="D60" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="61" spans="4:6">
+      <c r="D61" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="62" spans="4:6">
+      <c r="D62" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="63" spans="4:6">
+      <c r="D63" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="64" spans="4:6">
+      <c r="D64" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="65" spans="4:6">
+      <c r="D65" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="66" spans="4:6">
+      <c r="D66" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="67" spans="4:6">
+      <c r="D67" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="68" spans="4:6">
+      <c r="D68" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="69" spans="4:6">
+      <c r="D69" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="70" spans="4:6">
+      <c r="D70" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="71" spans="4:6">
+      <c r="D71" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="72" spans="4:6">
+      <c r="D72" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="73" spans="4:6">
+      <c r="D73" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="74" spans="4:6">
+      <c r="D74" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="75" spans="4:6">
+      <c r="D75" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="76" spans="4:6">
+      <c r="D76" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="77" spans="4:6">
+      <c r="D77" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="78" spans="4:6">
+      <c r="D78" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="79" spans="4:6">
+      <c r="D79" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="80" spans="4:6">
+      <c r="D80" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="81" spans="4:6">
+      <c r="D81" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="82" spans="4:6">
+      <c r="D82" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="83" spans="4:6">
+      <c r="D83" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="84" spans="4:6">
+      <c r="D84" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="85" spans="4:6">
+      <c r="D85" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="86" spans="4:6">
+      <c r="D86" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="87" spans="4:6">
+      <c r="D87" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="88" spans="4:6">
+      <c r="D88" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="89" spans="4:6">
+      <c r="D89" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="90" spans="4:6">
+      <c r="D90" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="91" spans="4:6">
+      <c r="D91" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="92" spans="4:6">
+      <c r="D92" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="93" spans="4:6">
+      <c r="D93" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="94" spans="4:6">
+      <c r="D94" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="95" spans="4:6">
+      <c r="D95" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="96" spans="4:6">
+      <c r="D96" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="97" spans="4:6">
+      <c r="D97" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="98" spans="4:6">
+      <c r="D98" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="99" spans="4:6">
+      <c r="D99" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="100" spans="4:6">
+      <c r="D100" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="101" spans="4:6">
+      <c r="F101" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>